<commit_message>
2017-03-18: 1. webpack done 2. gulp done
</commit_message>
<xml_diff>
--- a/doc/package.xlsx
+++ b/doc/package.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13050"/>
+    <workbookView windowWidth="28695" windowHeight="12630" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="node" sheetId="1" r:id="rId1"/>
+    <sheet name="gulp" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43">
   <si>
     <t>express</t>
   </si>
@@ -55,6 +55,96 @@
   </si>
   <si>
     <t>https://github.com/cure53/DOMPurify</t>
+  </si>
+  <si>
+    <t>名称</t>
+  </si>
+  <si>
+    <t>作用</t>
+  </si>
+  <si>
+    <t>安装</t>
+  </si>
+  <si>
+    <t>实例</t>
+  </si>
+  <si>
+    <t>gulp-htmlmin</t>
+  </si>
+  <si>
+    <t>压缩html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">npm install gulp-htmlmin --save-dev </t>
+  </si>
+  <si>
+    <t>http://blog.csdn.net/zhongguohaoshaonian/article/details/53207254</t>
+  </si>
+  <si>
+    <t>gulp-load-plugins</t>
+  </si>
+  <si>
+    <t>用$代替require，直接引用一个插件</t>
+  </si>
+  <si>
+    <t xml:space="preserve">npm install gulp-load-plugins --save-dev </t>
+  </si>
+  <si>
+    <t>https://juejin.im/entry/55c8dbb160b22a3ebdf34d57</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> gulp-uglify</t>
+  </si>
+  <si>
+    <t>压缩js</t>
+  </si>
+  <si>
+    <t>npm install --save-dev gulp-uglify</t>
+  </si>
+  <si>
+    <t>pump</t>
+  </si>
+  <si>
+    <t>捕获pipe中的error并显示</t>
+  </si>
+  <si>
+    <t>npm install --save-dev pump</t>
+  </si>
+  <si>
+    <t>gulp-minify-css</t>
+  </si>
+  <si>
+    <t>压缩css</t>
+  </si>
+  <si>
+    <t>npm install --save-dev gulp-minify-css</t>
+  </si>
+  <si>
+    <t>gulp-concat</t>
+  </si>
+  <si>
+    <t>合并文件</t>
+  </si>
+  <si>
+    <t>npm install --save-dev gulp-concat</t>
+  </si>
+  <si>
+    <t>gulp-babel</t>
+  </si>
+  <si>
+    <t>babel</t>
+  </si>
+  <si>
+    <t>npm install --save-dev gulp-babel</t>
+  </si>
+  <si>
+    <t>gulp-rename</t>
+  </si>
+  <si>
+    <t>重新命名文件</t>
+  </si>
+  <si>
+    <t>npm install --save-dev gulp-rename</t>
   </si>
 </sst>
 </file>
@@ -62,10 +152,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -668,9 +758,10 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1017,8 +1108,8 @@
   <sheetPr/>
   <dimension ref="A2:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="3"/>
@@ -1060,7 +1151,7 @@
       <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1074,7 +1165,7 @@
       <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1092,14 +1183,131 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="19.375" customWidth="1"/>
+    <col min="3" max="3" width="42.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="http://blog.csdn.net/zhongguohaoshaonian/article/details/53207254"/>
+    <hyperlink ref="D3" r:id="rId2" display="https://juejin.im/entry/55c8dbb160b22a3ebdf34d57"/>
+  </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
2017-05-04: optimize arch: 1. use part. 2. simplify HTTP operation
</commit_message>
<xml_diff>
--- a/doc/package.xlsx
+++ b/doc/package.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44">
   <si>
     <t>express</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>npm install --save-dev gulp-rename</t>
+  </si>
+  <si>
+    <t>npm install --save-dev axios</t>
   </si>
 </sst>
 </file>
@@ -152,10 +155,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -288,23 +291,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -325,6 +328,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -337,30 +364,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -373,48 +376,48 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -433,6 +436,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -445,7 +484,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,48 +503,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -616,10 +619,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -628,115 +631,115 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -745,13 +748,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -760,7 +763,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1183,10 +1186,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C4"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
@@ -1301,6 +1304,11 @@
       </c>
       <c r="C9" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3">
+      <c r="C22" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>